<commit_message>
feat: fixed pivot stuff
</commit_message>
<xml_diff>
--- a/Assets/Resources/Levels/Halloween Game Jam 2025 (1).xlsx
+++ b/Assets/Resources/Levels/Halloween Game Jam 2025 (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\BLO.OD.-PAC.T\Assets\Resources\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828DCB91-CA91-4C7C-A1EC-9C4A3A1F9F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC3D25B-CE6E-45E1-887C-B41B99232B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task1.1" sheetId="21" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="100">
   <si>
     <t>`</t>
   </si>
@@ -1786,7 +1786,7 @@
   <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2076,9 +2076,6 @@
       </c>
       <c r="F11" s="111" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>0</v>
       </c>
       <c r="N11" s="30" t="s">
         <v>5</v>
@@ -3096,8 +3093,8 @@
   </sheetPr>
   <dimension ref="A1:AE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3526,9 +3523,6 @@
       <c r="C16" s="2"/>
       <c r="D16" s="64"/>
       <c r="E16" s="3"/>
-      <c r="F16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="30" t="s">
         <v>5</v>
       </c>
@@ -3633,8 +3627,8 @@
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4085,9 +4079,6 @@
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="45"/>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
       <c r="N17" s="30"/>
       <c r="O17" s="31"/>
       <c r="P17" s="32"/>
@@ -5000,7 +4991,7 @@
   <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5472,9 +5463,7 @@
   </sheetPr>
   <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5867,9 +5856,6 @@
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="45"/>
-      <c r="E16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="30" t="s">
         <v>5</v>
       </c>
@@ -6634,7 +6620,7 @@
   <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7538,7 +7524,7 @@
   <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8024,9 +8010,6 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
-      <c r="K16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="30" t="s">
         <v>33</v>
       </c>
@@ -8320,8 +8303,8 @@
   </sheetPr>
   <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8662,9 +8645,6 @@
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
       <c r="B16" s="113"/>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="37" t="s">
         <v>5</v>
       </c>
@@ -8797,7 +8777,7 @@
   <dimension ref="A1:AE27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9085,9 +9065,6 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
-      <c r="K16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="37" t="s">
         <v>5</v>
       </c>
@@ -9237,7 +9214,7 @@
   <dimension ref="A1:AE28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9624,9 +9601,6 @@
       <c r="H17" s="64"/>
       <c r="I17" s="64"/>
       <c r="J17" s="72"/>
-      <c r="K17" t="s">
-        <v>0</v>
-      </c>
       <c r="N17" s="30"/>
       <c r="O17" s="31"/>
       <c r="P17" s="32"/>
@@ -10923,7 +10897,7 @@
   <dimension ref="A1:AE23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11364,7 +11338,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11541,9 +11515,6 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="3"/>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
       <c r="N12" s="30" t="s">
         <v>5</v>
       </c>
@@ -12043,8 +12014,8 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12275,9 +12246,6 @@
       <c r="D16" s="2"/>
       <c r="E16" s="14"/>
       <c r="F16" s="3"/>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="103" t="s">
         <v>5</v>
       </c>
@@ -12424,7 +12392,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12661,9 +12629,6 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="30" t="s">
         <v>5</v>
       </c>
@@ -12815,7 +12780,9 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -13039,9 +13006,6 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="30" t="s">
         <v>5</v>
       </c>
@@ -13496,7 +13460,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13737,9 +13701,6 @@
       <c r="D16" s="2"/>
       <c r="E16" s="14"/>
       <c r="F16" s="3"/>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
       <c r="N16" s="30" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
feat: json null color accurate
</commit_message>
<xml_diff>
--- a/Assets/Resources/Levels/Halloween Game Jam 2025 (1).xlsx
+++ b/Assets/Resources/Levels/Halloween Game Jam 2025 (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard\BLO.OD.-PAC.T\Assets\Resources\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC3D25B-CE6E-45E1-887C-B41B99232B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26529688-6E9B-4273-BE0F-AED63DA48716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="15" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Task1.1" sheetId="21" r:id="rId1"/>
@@ -830,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1034,6 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5463,7 +5464,9 @@
   </sheetPr>
   <dimension ref="A1:AE23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -5835,6 +5838,12 @@
       <c r="B15" t="s">
         <v>0</v>
       </c>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
       <c r="N15" s="37" t="s">
         <v>5</v>
       </c>
@@ -5856,6 +5865,12 @@
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="45"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="115"/>
+      <c r="H16" s="115"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
       <c r="N16" s="30" t="s">
         <v>5</v>
       </c>
@@ -5872,6 +5887,12 @@
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="D17" s="46"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="115"/>
       <c r="N17" s="30"/>
       <c r="O17" s="31"/>
       <c r="P17" s="31"/>
@@ -5880,6 +5901,12 @@
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="D18" s="46"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="115"/>
+      <c r="G18" s="115"/>
+      <c r="H18" s="115"/>
+      <c r="I18" s="115"/>
+      <c r="J18" s="115"/>
       <c r="N18" s="37" t="s">
         <v>33</v>
       </c>
@@ -5894,6 +5921,12 @@
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="D19" s="46"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="115"/>
+      <c r="I19" s="115"/>
+      <c r="J19" s="115"/>
       <c r="N19" s="37" t="s">
         <v>33</v>
       </c>
@@ -5912,6 +5945,12 @@
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="47"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="115"/>
       <c r="N20" s="30" t="s">
         <v>33</v>
       </c>
@@ -5926,12 +5965,24 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="115"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="115"/>
       <c r="N21" s="30"/>
       <c r="O21" s="31"/>
       <c r="P21" s="31"/>
       <c r="Q21" s="32"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="115"/>
       <c r="N22" s="30" t="s">
         <v>5</v>
       </c>
@@ -7001,7 +7052,7 @@
   <dimension ref="A1:AE22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8303,7 +8354,7 @@
   </sheetPr>
   <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -8776,7 +8827,7 @@
   </sheetPr>
   <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -9213,8 +9264,8 @@
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>